<commit_message>
Dodane engleske Excelice za "Record of processing activities"
(cherry picked from commit 05b4609f1ed8477ff12fdba348fec5a168a5e526)
</commit_message>
<xml_diff>
--- a/assets/excel/en/ps_export_template_rpadp.xlsx
+++ b/assets/excel/en/ps_export_template_rpadp.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6041B26-34E2-4FEF-8DF3-18DBF2A06869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81D410C-99F0-496C-9BF0-EFB7F79D4D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{38079957-6A62-4BF1-94FC-1E6108123746}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{38079957-6A62-4BF1-94FC-1E6108123746}"/>
   </bookViews>
   <sheets>
     <sheet name="Evidencija" sheetId="6" r:id="rId1"/>
@@ -25,76 +25,76 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
-    <t>OPIS PODUZETIH SIGURNOSNIH MJERA U SLUČAJU PRIJENOSA PODATAKA U TREĆE ZEMLJE</t>
-  </si>
-  <si>
-    <t>NAPOMENE</t>
-  </si>
-  <si>
-    <t>Važne činjenice koje nisu obuhvaćene
-prethodnim kategorijama</t>
-  </si>
-  <si>
-    <t>TELEFON:</t>
-  </si>
-  <si>
     <t>EMAIL:</t>
   </si>
   <si>
-    <t>ADRESA:</t>
-  </si>
-  <si>
-    <t>NAZIV:</t>
-  </si>
-  <si>
-    <t>IME I PREZIME:</t>
-  </si>
-  <si>
-    <t>Službenik za zaštitu podataka (ukoliko je imenovan)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Podaci o izvršitelju obrade </t>
-  </si>
-  <si>
-    <t>VODITELJ OBRADE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poveznica na ugovor s voditeljem obrade </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAZIV I KONTAKT PODACI VODITELJA OBRADE  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SLUŽBENIK ZA ZAŠTITU PODATAKA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Naziv voditelja obrade/ime, ulica i broj, mjesto, broj telefona, e-mail </t>
-  </si>
-  <si>
-    <t>Naziv/ime, pozicija tj. Radno mjesto/vanjski, ulica i broj, mjesto, broj telefona, e-mail 
-(ako postoji)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KATEGORIJE (POSTUPCI/VRSTE) OBRADE </t>
-  </si>
-  <si>
-    <t>PRIJENOSI OSOBNIH PODATAKA U TREĆU ZEMLJU ILI MEĐUNARODNU ORGANIZACIJU
-(LOKACIJA OSOBNIH PODATAKA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPIS TEHNIČKIH I ORGANIZACIJSKIH SIGURNOSNIH MJERA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Opisati tehničke i organzacijske sigurnosne mjere primijenjene/odnosne na predmetnu obradu osobnih podataka </t>
-  </si>
-  <si>
-    <t>Navesti kategorije (postupke/vrste) obrade osobnih podataka koje se obavljaju u ime/za voditelja obrade</t>
-  </si>
-  <si>
-    <t>Naziv treće zemlje ili međunarodne organizacije (uključivo i podaci o primatelju/ima)                               Poveznica na dokumentaciju o adekvatnosti tj. odgovarajućim zaštitnim mjerama</t>
-  </si>
-  <si>
-    <t>Npr. standardne ugovorne klauzule ili obvezujuća korporativna pravila  (*poglavlje V GDPR-a). Ako postoji prijenost osobnih podataka u treće zemlje, staviti poveznicu na dokumente kojima su takvi prijenosi regulirani</t>
+    <t xml:space="preserve">Information about the processor </t>
+  </si>
+  <si>
+    <t>Data Protection Officer (if designated)</t>
+  </si>
+  <si>
+    <t>NAME:</t>
+  </si>
+  <si>
+    <t>ADDRESS:</t>
+  </si>
+  <si>
+    <t>TELEPHONE:</t>
+  </si>
+  <si>
+    <t>NAME AND SURNAME:</t>
+  </si>
+  <si>
+    <t>CONTROLLER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME AND CONTACT DETAILS OF THE CONTROLLER  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATA PROTECTION OFFICER </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CATEGORIES (PROCEDURES/TYPES) OF PROCESSING </t>
+  </si>
+  <si>
+    <t>TRANSFERS OF PERSONAL DATA TO A THIRD COUNTRY OR TO AN INTERNATIONAL ORGANISATION
+(LOCATION OF PERSONAL DATA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESCRIPTION OF TECHNICAL AND ORGANISATIONAL SECURITY MEASURES </t>
+  </si>
+  <si>
+    <t>DESCRIPTION OF THE SECURITY MEASURES TAKEN IN CASE OF DATA TRANSFERS TO THIRD COUNTRIES</t>
+  </si>
+  <si>
+    <t>REMARKS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Link to the contract with the controller </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of the controller/name, street and number, place, telephone number, e-mail </t>
+  </si>
+  <si>
+    <t>Name/name, position i.e. workplace, street and number, place, telephone number, e-mail 
+(if any)</t>
+  </si>
+  <si>
+    <t>Specify the categories (procedures/types) of the processing of personal data carried out on behalf of the controller</t>
+  </si>
+  <si>
+    <t>Name of the third country or international organisation (including the recipient’s details) Link to the adequacy decision documentation, i.e. appropriate safeguards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describe the technical and organisational security measures applied to the processing of personal data in question </t>
+  </si>
+  <si>
+    <t>E.g. Standard Contractual Clauses or Binding Corporate Rules (Article 49 of the GDPR ). Where there is a transfer of personal data to third countries, provide a link to the documents governing such transfers;</t>
+  </si>
+  <si>
+    <t>Important facts not covered
+previous categories</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -522,7 +522,7 @@
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -562,7 +562,7 @@
           <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -602,7 +602,7 @@
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -642,7 +642,7 @@
           <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -682,7 +682,7 @@
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -695,6 +695,13 @@
         </top>
         <bottom style="thin">
           <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="hair">
+          <color theme="2"/>
         </bottom>
       </border>
     </dxf>
@@ -729,14 +736,7 @@
           <bgColor theme="0" tint="-0.249977111117893"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="hair">
-          <color theme="2"/>
-        </bottom>
-      </border>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
       <font>
@@ -762,7 +762,7 @@
           <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="2"/>
@@ -788,15 +788,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A38C48B1-5664-4B65-A3DE-3964409854A0}" name="Tablica13" displayName="Tablica13" ref="C7:H8" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
-  <autoFilter ref="C7:H8" xr:uid="{A38C48B1-5664-4B65-A3DE-3964409854A0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{24B51D83-0792-447C-AADB-D5A5A6D9BC89}" name="Tablica132" displayName="Tablica132" ref="C7:H8" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7">
+  <autoFilter ref="C7:H8" xr:uid="{24B51D83-0792-447C-AADB-D5A5A6D9BC89}"/>
   <tableColumns count="6">
-    <tableColumn id="3" xr3:uid="{384C2D93-3B06-479B-86C3-F7AF3C8AA286}" name="SLUŽBENIK ZA ZAŠTITU PODATAKA " dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{16D380C0-F94B-421A-B0A8-FAD43DFF8B0E}" name="KATEGORIJE (POSTUPCI/VRSTE) OBRADE " dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{72474BB4-779B-4B72-92B8-3B0361C2D5E3}" name="PRIJENOSI OSOBNIH PODATAKA U TREĆU ZEMLJU ILI MEĐUNARODNU ORGANIZACIJU_x000a_(LOKACIJA OSOBNIH PODATAKA)" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{1D3E3217-24C1-40B8-9AF3-D2BCB1542DD3}" name="OPIS TEHNIČKIH I ORGANIZACIJSKIH SIGURNOSNIH MJERA " dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{1077DFCE-9FC3-403A-AE5C-E4592D39857C}" name="OPIS PODUZETIH SIGURNOSNIH MJERA U SLUČAJU PRIJENOSA PODATAKA U TREĆE ZEMLJE" dataDxfId="1"/>
-    <tableColumn id="15" xr3:uid="{E5834379-9434-4385-9AB9-AD7B05E12D9C}" name="NAPOMENE" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{94E7E5FC-F8E6-4699-A65F-D2031BDDD086}" name="SLUŽBENIK ZA ZAŠTITU PODATAKA " dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{C7484536-E741-4A90-842B-4218B23B5C5B}" name="KATEGORIJE (POSTUPCI/VRSTE) OBRADE " dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{6069A1C6-8E51-43E0-B0BE-3D38C1D855AF}" name="PRIJENOSI OSOBNIH PODATAKA U TREĆU ZEMLJU ILI MEĐUNARODNU ORGANIZACIJU_x000a_(LOKACIJA OSOBNIH PODATAKA)" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{0AF073B9-0C1E-44E1-9C12-4A822BC74B3D}" name="OPIS TEHNIČKIH I ORGANIZACIJSKIH SIGURNOSNIH MJERA " dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{ED64CA99-69CB-485B-BA07-DE1C0DA03384}" name="OPIS PODUZETIH SIGURNOSNIH MJERA U SLUČAJU PRIJENOSA PODATAKA U TREĆE ZEMLJE" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{6408498D-D96C-498A-A9F6-6DD4580C5EAB}" name="NAPOMENE" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1105,93 +1105,93 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7265625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="17" style="4" customWidth="1"/>
     <col min="3" max="3" width="18" style="23" customWidth="1"/>
-    <col min="4" max="4" width="27.54296875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="29.453125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="56.26953125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="28.453125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="26.26953125" style="23" customWidth="1"/>
-    <col min="9" max="16384" width="8.81640625" style="4"/>
+    <col min="4" max="4" width="27.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="56.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" style="23" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="30" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C1" s="30"/>
       <c r="D1" s="31" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E1" s="31"/>
       <c r="F1" s="2"/>
       <c r="G1" s="3"/>
       <c r="H1" s="24"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="16" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="25"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="25"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="16" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="25"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="16" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="25"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="21"/>
       <c r="C6" s="8"/>
@@ -1203,58 +1203,58 @@
     </row>
     <row r="7" spans="1:9" s="14" customFormat="1" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="E7" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="G7" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="26" t="s">
-        <v>0</v>
-      </c>
       <c r="H7" s="26" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="14" customFormat="1" ht="97.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D8" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="G8" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="27" t="s">
+      <c r="H8" s="27" t="s">
         <v>22</v>
-      </c>
-      <c r="H8" s="27" t="s">
-        <v>2</v>
       </c>
       <c r="I8" s="15"/>
     </row>
-    <row r="9" spans="1:9" s="14" customFormat="1" ht="10.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A9" s="19"/>
       <c r="B9" s="18"/>
       <c r="C9" s="29"/>
@@ -1265,7 +1265,7 @@
       <c r="H9" s="28"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="22"/>

</xml_diff>